<commit_message>
score_brief script and the reference lookup scripts
</commit_message>
<xml_diff>
--- a/data-raw/brief2_scoringtables.xlsx
+++ b/data-raw/brief2_scoringtables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azp271/OneDrive - The Pennsylvania State University/b-childfoodlab_Shared/Active_Studies/kellertools/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365.sharepoint.com/sites/b-childfoodlab/Shared Documents/Box Migration Data/b-childfoodlab_Shared/Active_Studies/kellertools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C7C01171-D28A-C346-B382-0BBBD019FC01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{753953DD-E9AC-114C-957D-E1AE00415A8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boys5-7" sheetId="8" r:id="rId1"/>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>subscale_raw</t>
-  </si>
-  <si>
-    <t>inhbit_t</t>
-  </si>
-  <si>
-    <t>inhbit_p</t>
   </si>
   <si>
     <t>selfmon_t</t>
@@ -137,11 +131,17 @@
   <si>
     <t>gec_raw</t>
   </si>
+  <si>
+    <t>inhibit_t</t>
+  </si>
+  <si>
+    <t>inhibit_p</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -614,11 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,88 +632,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -7850,11 +7850,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7868,88 +7868,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -15086,11 +15086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15104,88 +15104,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -22322,11 +22322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22340,88 +22340,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -29558,11 +29558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29576,88 +29576,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -36793,11 +36793,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36811,88 +36811,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -44029,11 +44029,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44047,88 +44047,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -51264,11 +51264,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AC146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51282,88 +51282,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -58497,4 +58497,272 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="054cdb9d99f894db796ababf7b791478">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c10d8bc434365a681a376bfc5a38d7dd" ns2:_="" ns3:_="">
+    <xsd:import namespace="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
+    <xsd:import namespace="cf6faeb8-54d1-4580-a175-bd3097eaab2a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf6faeb8-54d1-4580-a175-bd3097eaab2a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B32447E8-BD2E-4D98-9D0D-DC00E1716B60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A23581CC-6511-4A1D-A23E-51B17AB36DFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03673BCD-2A49-486E-9376-1C9FF7D5F33E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
+    <ds:schemaRef ds:uri="cf6faeb8-54d1-4580-a175-bd3097eaab2a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
addition of microstructure database processing
</commit_message>
<xml_diff>
--- a/data-raw/brief2_scoringtables.xlsx
+++ b/data-raw/brief2_scoringtables.xlsx
@@ -58501,7 +58501,12 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf6faeb8-54d1-4580-a175-bd3097eaab2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -58515,8 +58520,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="054cdb9d99f894db796ababf7b791478">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c10d8bc434365a681a376bfc5a38d7dd" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7862d82d44fe1e1057ec1095428d9d1e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa7f64b43084f2101da197942b16f334" ns2:_="" ns3:_="">
     <xsd:import namespace="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
     <xsd:import namespace="cf6faeb8-54d1-4580-a175-bd3097eaab2a"/>
     <xsd:element name="properties">
@@ -58537,6 +58542,9 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -58572,6 +58580,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{14738273-d04b-4d91-a371-b3953d63e64a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf6faeb8-54d1-4580-a175-bd3097eaab2a" elementFormDefault="qualified">
@@ -58630,6 +58649,18 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="28b28469-8996-4088-bd89-44d87d6385e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -58749,20 +58780,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03673BCD-2A49-486E-9376-1C9FF7D5F33E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
-    <ds:schemaRef ds:uri="cf6faeb8-54d1-4580-a175-bd3097eaab2a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0FAD2F-42D0-4E20-8486-120FDD038E19}"/>
 </file>
</xml_diff>

<commit_message>
updated child3_lab to fix bis/bas response codign (backwards in Qualtrics), updated inherit_param from fbs_intake to fbs_kcal_intake, and recompiled package
</commit_message>
<xml_diff>
--- a/data-raw/brief2_scoringtables.xlsx
+++ b/data-raw/brief2_scoringtables.xlsx
@@ -58520,8 +58520,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7862d82d44fe1e1057ec1095428d9d1e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa7f64b43084f2101da197942b16f334" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29caeb97e587edc5ffd97c0cc955b9a0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="125c276e8ad9ac2088d73c59cf4fd2f7" ns2:_="" ns3:_="">
     <xsd:import namespace="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
     <xsd:import namespace="cf6faeb8-54d1-4580-a175-bd3097eaab2a"/>
     <xsd:element name="properties">
@@ -58545,6 +58545,7 @@
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -58661,6 +58662,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -58780,5 +58786,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0FAD2F-42D0-4E20-8486-120FDD038E19}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF3401E9-F54F-4471-AA45-3E795F188763}"/>
 </file>
</xml_diff>